<commit_message>
Se realizan solicitados en kanban para dar formato la presentacion
</commit_message>
<xml_diff>
--- a/Insumos/diccionario_edomex_enero_2025.xlsx
+++ b/Insumos/diccionario_edomex_enero_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Shared drives\Morant Consultores\Clientes\CesarFaz_EdoMex\Encuesta\2025\Enero\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1E22FB-9495-4A25-9EAE-95A6BCD4F226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95885C4-6ACB-407D-8DC8-D0BD8D4F10C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2115" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="315">
   <si>
     <t>bloque</t>
   </si>
@@ -717,9 +717,6 @@
     <t>conoce_per2_horacio</t>
   </si>
   <si>
-    <t>Horario Duarte</t>
-  </si>
-  <si>
     <t>¿Cuál es su opinión sobre (...), buena o mala?</t>
   </si>
   <si>
@@ -981,6 +978,15 @@
   </si>
   <si>
     <t>programa_social_o3</t>
+  </si>
+  <si>
+    <t>Estado de México</t>
+  </si>
+  <si>
+    <t>Su Municipio</t>
+  </si>
+  <si>
+    <t>Horacio Duarte</t>
   </si>
 </sst>
 </file>
@@ -1354,9 +1360,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D109" sqref="D109:D111"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G96" sqref="G96:G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3582,7 +3588,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="5" t="s">
-        <v>126</v>
+        <v>312</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>127</v>
@@ -3624,7 +3630,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="5" t="s">
-        <v>126</v>
+        <v>313</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>127</v>
@@ -5300,7 +5306,7 @@
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3" t="s">
-        <v>225</v>
+        <v>314</v>
       </c>
       <c r="H96" s="5" t="s">
         <v>41</v>
@@ -5331,23 +5337,23 @@
         <v>222</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>224</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3" t="s">
-        <v>225</v>
+        <v>314</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
@@ -5375,20 +5381,20 @@
         <v>222</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>224</v>
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="3" t="s">
-        <v>225</v>
+        <v>314</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -5414,22 +5420,22 @@
     </row>
     <row r="99" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B99" s="10" t="s">
         <v>231</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="8"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
@@ -5454,22 +5460,22 @@
     </row>
     <row r="100" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
@@ -5494,24 +5500,24 @@
     </row>
     <row r="101" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B101" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B101" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="8"/>
       <c r="G101" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H101" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
@@ -5536,24 +5542,24 @@
     </row>
     <row r="102" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B102" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B102" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8"/>
       <c r="G102" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
@@ -5578,24 +5584,24 @@
     </row>
     <row r="103" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B103" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
       <c r="G103" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
@@ -5620,24 +5626,24 @@
     </row>
     <row r="104" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B104" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B104" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="8"/>
       <c r="G104" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
@@ -5662,24 +5668,24 @@
     </row>
     <row r="105" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B105" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B105" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E105" s="8"/>
       <c r="F105" s="8"/>
       <c r="G105" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
@@ -5704,24 +5710,24 @@
     </row>
     <row r="106" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B106" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B106" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
       <c r="G106" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
@@ -5746,24 +5752,24 @@
     </row>
     <row r="107" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B107" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
       <c r="G107" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
@@ -5788,24 +5794,24 @@
     </row>
     <row r="108" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B108" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B108" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
       <c r="G108" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
@@ -5830,22 +5836,22 @@
     </row>
     <row r="109" spans="1:28" s="21" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C109" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D109" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E109" s="17"/>
       <c r="F109" s="17"/>
       <c r="G109" s="17"/>
       <c r="H109" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I109" s="17"/>
       <c r="J109" s="17"/>
@@ -5870,22 +5876,22 @@
     </row>
     <row r="110" spans="1:28" s="21" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C110" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D110" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E110" s="17"/>
       <c r="F110" s="17"/>
       <c r="G110" s="17"/>
       <c r="H110" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I110" s="17"/>
       <c r="J110" s="17"/>
@@ -5910,22 +5916,22 @@
     </row>
     <row r="111" spans="1:28" s="21" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C111" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D111" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E111" s="17"/>
       <c r="F111" s="17"/>
       <c r="G111" s="17"/>
       <c r="H111" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I111" s="17"/>
       <c r="J111" s="17"/>
@@ -5950,22 +5956,22 @@
     </row>
     <row r="112" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B112" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="B112" s="10" t="s">
-        <v>259</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
@@ -5990,22 +5996,22 @@
     </row>
     <row r="113" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
@@ -6030,16 +6036,16 @@
     </row>
     <row r="114" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
@@ -6070,22 +6076,22 @@
     </row>
     <row r="115" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
       <c r="G115" s="7"/>
       <c r="H115" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
@@ -6110,22 +6116,22 @@
     </row>
     <row r="116" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
       <c r="G116" s="7"/>
       <c r="H116" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
@@ -6150,16 +6156,16 @@
     </row>
     <row r="117" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
@@ -6188,22 +6194,22 @@
     </row>
     <row r="118" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
       <c r="G118" s="7"/>
       <c r="H118" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
@@ -6228,22 +6234,22 @@
     </row>
     <row r="119" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B119" s="11" t="s">
         <v>278</v>
-      </c>
-      <c r="B119" s="11" t="s">
-        <v>279</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
       <c r="G119" s="7"/>
       <c r="H119" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
@@ -6268,22 +6274,22 @@
     </row>
     <row r="120" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
       <c r="G120" s="4"/>
       <c r="H120" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
@@ -6308,22 +6314,22 @@
     </row>
     <row r="121" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
       <c r="G121" s="4"/>
       <c r="H121" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
@@ -6348,22 +6354,22 @@
     </row>
     <row r="122" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
       <c r="G122" s="4"/>
       <c r="H122" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
@@ -6388,22 +6394,22 @@
     </row>
     <row r="123" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
       <c r="G123" s="4"/>
       <c r="H123" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
@@ -6428,22 +6434,22 @@
     </row>
     <row r="124" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
       <c r="G124" s="4"/>
       <c r="H124" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
@@ -32830,10 +32836,10 @@
         <v>102</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>294</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32841,10 +32847,10 @@
         <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>296</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32852,10 +32858,10 @@
         <v>104</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>298</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32863,10 +32869,10 @@
         <v>105</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>300</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32874,10 +32880,10 @@
         <v>106</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>302</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32885,10 +32891,10 @@
         <v>107</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32896,10 +32902,10 @@
         <v>108</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>306</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -32907,10 +32913,10 @@
         <v>109</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>308</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>